<commit_message>
[Feat] : Excel로 .proto 파일 만드는 기능 추가
- 앞에 CS_, SC_가 붙은 MessageName은 PacketID를 생성하고, 그렇지 않은 MessageName들은 PacketID를 생성하지 않음
- 시트를 여러개 만들어도 상관없음
- 동일한 MessageName이 존재할 경우 오류 발생
</commit_message>
<xml_diff>
--- a/ProtoFileGenerator/dist/proto_definitions.xlsx
+++ b/ProtoFileGenerator/dist/proto_definitions.xlsx
@@ -5,23 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\Protobuf\PythonProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\ProtoFileGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F140C1-B3B4-4342-9E0A-CF2976C60C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3110E39-62F4-4582-A0D4-506C359D8DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="4185" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="3045" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
-    <sheet name="PacketEnum" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="78">
   <si>
     <t>MessageName</t>
   </si>
@@ -35,70 +34,226 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>SC_CreateMyCharacter</t>
+    <t>CS_ON_ACCEPT</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>최대 20자 유니코드 문자열 (실제 제한은 코드로 처리, 제한은 필요할때 늘리면 됨)</t>
+  </si>
+  <si>
+    <t>KDAInfo</t>
+  </si>
+  <si>
+    <t>kill</t>
+  </si>
+  <si>
+    <t>uint32</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>assist</t>
+  </si>
+  <si>
+    <t>PlayerInfo</t>
   </si>
   <si>
     <t>playerId</t>
   </si>
   <si>
-    <t>uint32</t>
-  </si>
-  <si>
-    <t>서버로부터 받은 ID</t>
+    <t>kda</t>
+  </si>
+  <si>
+    <t>SC_CREATE_MY_CHARACTER</t>
+  </si>
+  <si>
+    <t>서버로 부터 부여받은 ID</t>
   </si>
   <si>
     <t>posX</t>
   </si>
   <si>
-    <t>X 좌표</t>
+    <t>현재 위치</t>
   </si>
   <si>
     <t>posY</t>
   </si>
   <si>
-    <t>Y 좌표</t>
-  </si>
-  <si>
     <t>posZ</t>
   </si>
   <si>
-    <t>Z 좌표</t>
+    <t>dirX</t>
+  </si>
+  <si>
+    <t>보는 방향</t>
+  </si>
+  <si>
+    <t>dirY</t>
+  </si>
+  <si>
+    <t>dirZ</t>
   </si>
   <si>
     <t>maxHP</t>
   </si>
   <si>
-    <t>최대 체력</t>
-  </si>
-  <si>
-    <t>SC_CreateOtherCharacter</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>캐릭터 이름</t>
+    <t>최대 Hp</t>
+  </si>
+  <si>
+    <t>SC_CREATE_OTHER_CHARACTER</t>
+  </si>
+  <si>
+    <t>Hp</t>
   </si>
   <si>
     <t>curHP</t>
   </si>
   <si>
-    <t>현재 체력</t>
-  </si>
-  <si>
-    <t>PacketName</t>
-  </si>
-  <si>
-    <t>CS_OnAccept</t>
-  </si>
-  <si>
-    <t>SC_CharacterDown</t>
-  </si>
-  <si>
-    <t>SC_CharacterKillLog</t>
+    <t>이름</t>
+  </si>
+  <si>
+    <t>kdaInfo</t>
+  </si>
+  <si>
+    <t>KDA 정보</t>
+  </si>
+  <si>
+    <t>SC_CHARACTER_DOWN</t>
+  </si>
+  <si>
+    <t>SC_CHARACTER_KILL_LOG</t>
+  </si>
+  <si>
+    <t>playerInfoList</t>
+  </si>
+  <si>
+    <t>repeated PlayerInfo</t>
+  </si>
+  <si>
+    <t>모든 플레이어들의 KDA 정보</t>
+  </si>
+  <si>
+    <t>CS_KEY_INPUT</t>
+  </si>
+  <si>
+    <t>keyW</t>
+  </si>
+  <si>
+    <t>키(WASD)</t>
+  </si>
+  <si>
+    <t>keyA</t>
+  </si>
+  <si>
+    <t>keyS</t>
+  </si>
+  <si>
+    <t>keyD</t>
+  </si>
+  <si>
+    <t>rotateAxisX</t>
+  </si>
+  <si>
+    <t>fixed32</t>
+  </si>
+  <si>
+    <t>마우스 X축 회전값</t>
+  </si>
+  <si>
+    <t>rotateAxisY</t>
+  </si>
+  <si>
+    <t>마우스 Y축 회전값</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>점프 여부</t>
+  </si>
+  <si>
+    <t>SC_KEY_INPUT</t>
+  </si>
+  <si>
+    <t>CS_POS_INTERPOLATION</t>
+  </si>
+  <si>
+    <t>플레이어의 현재 위치</t>
+  </si>
+  <si>
+    <t>SC_POS_INTERPOLATION</t>
+  </si>
+  <si>
+    <t>CS_ATTACK</t>
+  </si>
+  <si>
+    <t>bAttack</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>임의의 변수, 의미 없음.</t>
+  </si>
+  <si>
+    <t>SC_ATTACK</t>
+  </si>
+  <si>
+    <t>CS_SHOT_HIT</t>
+  </si>
+  <si>
+    <t>피격 대상</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>피격 대상의 남은 HP</t>
+  </si>
+  <si>
+    <t>SC_SHOT_HIT</t>
+  </si>
+  <si>
+    <t>CS_THROW_GRENADE</t>
+  </si>
+  <si>
+    <t>던지기 시작 위치</t>
+  </si>
+  <si>
+    <t>던지는 방향</t>
+  </si>
+  <si>
+    <t>SC_THROW_GRENADE</t>
+  </si>
+  <si>
+    <t>CS_GRENADE_EXPLOSITION_POS</t>
+  </si>
+  <si>
+    <t>터질 위치</t>
+  </si>
+  <si>
+    <t>SC_GRENADEEXPLOSITIONPOS</t>
+  </si>
+  <si>
+    <t>CS_CHANGE_WEAPON</t>
+  </si>
+  <si>
+    <t>weapon</t>
+  </si>
+  <si>
+    <t>무기 교체</t>
+  </si>
+  <si>
+    <t>SC_CHANGE_WEAPON</t>
+  </si>
+  <si>
+    <t>다른 캐릭터 ID</t>
   </si>
 </sst>
 </file>
@@ -470,18 +625,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -512,146 +667,953 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
         <v>21</v>
       </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C74" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C75" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" t="s">
         <v>25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>69</v>
+      </c>
+      <c r="B80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>69</v>
+      </c>
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>72</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>72</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>73</v>
+      </c>
+      <c r="B93" t="s">
+        <v>74</v>
+      </c>
+      <c r="C93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>76</v>
+      </c>
+      <c r="B96" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>